<commit_message>
Sensor and Wireless Charging Calculations
Random Sensor and Wireless Charging Applications
</commit_message>
<xml_diff>
--- a/Projects/Wireless_Charging/Wireless_Charging-Calculations-X01.xlsx
+++ b/Projects/Wireless_Charging/Wireless_Charging-Calculations-X01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carld\Documents\GitHub\GT-BITNG\Projects\Wireless_Charging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0139BB-0CE2-4E9B-9B35-CCC130F0C63B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E930B692-5E1B-49A0-A127-44DD4D15AAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2CFCA7FC-FEC4-4172-80EE-2DB86B4F0902}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,15 +661,15 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <f>((($B$11*2*PI())^2*B5)^-1)*1000000000</f>
+        <f t="shared" ref="B7:I7" si="0">((($B$11*2*PI())^2*B5)^-1)*1000000000</f>
         <v>23.453977694985603</v>
       </c>
       <c r="C7" s="1">
-        <f>((($B$11*2*PI())^2*C5)^-1)*1000000000</f>
+        <f t="shared" si="0"/>
         <v>19.913754646685888</v>
       </c>
       <c r="D7" s="1">
-        <f>((($B$11*2*PI())^2*D5)^-1)*1000000000</f>
+        <f t="shared" si="0"/>
         <v>76.112668000554223</v>
       </c>
       <c r="E7" s="1">
@@ -677,19 +677,19 @@
         <v>53.665881166492468</v>
       </c>
       <c r="F7" s="1">
-        <f>((($B$11*2*PI())^2*F5)^-1)*1000000000</f>
+        <f t="shared" si="0"/>
         <v>50.258523632112002</v>
       </c>
       <c r="G7" s="1">
-        <f>((($B$11*2*PI())^2*G5)^-1)*1000000000</f>
+        <f t="shared" si="0"/>
         <v>87.952416356196011</v>
       </c>
       <c r="H7" s="1">
-        <f>((($B$11*2*PI())^2*H5)^-1)*1000000000</f>
+        <f t="shared" si="0"/>
         <v>48.712107520354714</v>
       </c>
       <c r="I7" s="1">
-        <f>((($B$11*2*PI())^2*I5)^-1)*1000000000</f>
+        <f t="shared" si="0"/>
         <v>100.517047264224</v>
       </c>
     </row>
@@ -698,35 +698,35 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <f>(($B$12*2*PI())^2*B5-1/B7)^-1</f>
+        <f t="shared" ref="B8:I8" si="1">(($B$12*2*PI())^2*B5-1/B7)^-1</f>
         <v>9.3815910783695037E-10</v>
       </c>
       <c r="C8" s="1">
-        <f>(($B$12*2*PI())^2*C5-1/C7)^-1</f>
+        <f t="shared" si="1"/>
         <v>7.9655018589929732E-10</v>
       </c>
       <c r="D8" s="1">
-        <f>(($B$12*2*PI())^2*D5-1/D7)^-1</f>
+        <f t="shared" si="1"/>
         <v>3.0445067201439494E-9</v>
       </c>
       <c r="E8" s="1">
-        <f>(($B$12*2*PI())^2*E5-1/E7)^-1</f>
+        <f t="shared" si="1"/>
         <v>2.1466352467455643E-9</v>
       </c>
       <c r="F8" s="1">
-        <f>(($B$12*2*PI())^2*F5-1/F7)^-1</f>
+        <f t="shared" si="1"/>
         <v>2.0103409453648932E-9</v>
       </c>
       <c r="G8" s="1">
-        <f>(($B$12*2*PI())^2*G5-1/G7)^-1</f>
+        <f t="shared" si="1"/>
         <v>3.5180966543885636E-9</v>
       </c>
       <c r="H8" s="1">
-        <f>(($B$12*2*PI())^2*H5-1/H7)^-1</f>
+        <f t="shared" si="1"/>
         <v>1.9484843008921279E-9</v>
       </c>
       <c r="I8" s="1">
-        <f>(($B$12*2*PI())^2*I5-1/I7)^-1</f>
+        <f t="shared" si="1"/>
         <v>4.0206818907297865E-9</v>
       </c>
     </row>
@@ -735,35 +735,35 @@
         <v>0</v>
       </c>
       <c r="B9" s="1">
-        <f>(2*PI()*$B$11*B5/B6)</f>
+        <f t="shared" ref="B9:I9" si="2">(2*PI()*$B$11*B5/B6)</f>
         <v>30.844727871608868</v>
       </c>
       <c r="C9" s="1">
-        <f>(2*PI()*$B$11*C5/C6)</f>
+        <f t="shared" si="2"/>
         <v>29.821685487807581</v>
       </c>
       <c r="D9" s="1">
-        <f>(2*PI()*$B$11*D5/D6)</f>
+        <f t="shared" si="2"/>
         <v>11.005495106470349</v>
       </c>
       <c r="E9" s="1">
-        <f>(2*PI()*$B$11*E5/E6)</f>
+        <f t="shared" si="2"/>
         <v>19.771089766591764</v>
       </c>
       <c r="F9" s="1">
-        <f>(2*PI()*$B$11*F5/F6)</f>
+        <f t="shared" si="2"/>
         <v>46.569491100272224</v>
       </c>
       <c r="G9" s="1">
-        <f>(2*PI()*$B$11*G5/G6)</f>
+        <f t="shared" si="2"/>
         <v>20.563151914405914</v>
       </c>
       <c r="H9" s="1">
-        <f>(2*PI()*$B$11*H5/H6)</f>
+        <f t="shared" si="2"/>
         <v>40.8407044966673</v>
       </c>
       <c r="I9" s="1">
-        <f>(2*PI()*$B$11*I5/I6)</f>
+        <f t="shared" si="2"/>
         <v>63.334507896370226</v>
       </c>
     </row>
@@ -774,6 +774,10 @@
       <c r="B11" s="1">
         <v>200000</v>
       </c>
+      <c r="C11" s="1">
+        <f>1/(2*PI()*SQRT(0.000000047*0.00001215))</f>
+        <v>210611.97644978843</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -782,6 +786,22 @@
       <c r="B12" s="1">
         <f>1000000</f>
         <v>1000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="1">
+        <f>100/1.29</f>
+        <v>77.519379844961236</v>
+      </c>
+      <c r="E13" s="1">
+        <f>1/(2*PI()*SQRT(0.0000126*0.000000047))</f>
+        <v>206816.85521687404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="1">
+        <f>1/(2*PI()*SQRT(0.0000072*0.0000000033))</f>
+        <v>1032516.2929593984</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>